<commit_message>
Filled_orders.xlsx - temporary removal of the size variable
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/Filled_orders.xlsx
+++ b/src/main/resources/reports/Filled_orders.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Created at</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Volume</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;jt:forEach items="${table}" var="row"&gt;${row.created_ad}</t>
+    <t xml:space="preserve">&lt;jt:forEach items="${table}" var="row"&gt;${row.created_at}</t>
   </si>
   <si>
     <t xml:space="preserve">${row.trade_id}</t>
@@ -85,9 +85,6 @@
     <t xml:space="preserve">${row.price}</t>
   </si>
   <si>
-    <t xml:space="preserve">${row.size}</t>
-  </si>
-  <si>
     <t xml:space="preserve">${row.fee}</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">${row.settled}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$row.usd_volume}</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;/jt:forEach&gt;</t>
@@ -136,13 +130,13 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,80 +145,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9933"/>
-        <bgColor rgb="FFFFCC00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FFFF5050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
-        <bgColor rgb="FFFF6600"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0066"/>
-        <bgColor rgb="FFFF3399"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3399"/>
-        <bgColor rgb="FFFF33CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF33CC"/>
-        <bgColor rgb="FFFF3399"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC66FF"/>
-        <bgColor rgb="FF9966FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9966FF"/>
-        <bgColor rgb="FFCC66FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF6666FF"/>
-        <bgColor rgb="FF9966FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3366FF"/>
-        <bgColor rgb="FF6666FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0066CC"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF009999"/>
-        <bgColor rgb="FF008080"/>
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,60 +184,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,30 +206,30 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0066"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF33CC"/>
+      <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF009999"/>
+      <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9966FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF5050"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF3399"/>
+      <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
@@ -368,15 +242,15 @@
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC66FF"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9933"/>
+      <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF6666FF"/>
+      <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -395,16 +269,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>401760</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>606240</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>165240</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>368280</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>34920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -417,8 +291,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="21302400">
-          <a:off x="19433160" y="1650960"/>
-          <a:ext cx="6592680" cy="3502080"/>
+          <a:off x="18879840" y="2734560"/>
+          <a:ext cx="6597360" cy="3500640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,13 +312,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N172"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.78"/>
@@ -463,44 +337,44 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
@@ -525,25 +399,189 @@
       <c r="H2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>26</v>
-      </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Filled_orders.xlsx - shortend the columns width
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/Filled_orders.xlsx
+++ b/src/main/resources/reports/Filled_orders.xlsx
@@ -104,8 +104,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mmm\ d&quot;, &quot;yyyy"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="00"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -194,17 +201,65 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -284,67 +339,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="30.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="30.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="4" width="8.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="7.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="7.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="20.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -352,42 +406,52 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Filled_orders.xlsx - added usd_volume property to template
</commit_message>
<xml_diff>
--- a/src/main/resources/reports/Filled_orders.xlsx
+++ b/src/main/resources/reports/Filled_orders.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Created at</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">${row.settled}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${row.usd_volume}</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;/jt:forEach&gt;</t>
@@ -104,15 +107,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mmm\ d&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="00"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="171" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -226,39 +228,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,8 +343,8 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,10 +356,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="8.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="4" width="8.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="4" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="7.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="5" width="7.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="8.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="8.54"/>
   </cols>
   <sheetData>
@@ -439,8 +441,11 @@
       <c r="L2" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="M2" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="N2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>